<commit_message>
Sorted the orders of coordinates
</commit_message>
<xml_diff>
--- a/character9/character9_boxes_location.xlsx
+++ b/character9/character9_boxes_location.xlsx
@@ -462,376 +462,376 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>1</v>
+        <v>56</v>
       </c>
       <c r="B2" t="n">
-        <v>686</v>
+        <v>847</v>
       </c>
       <c r="C2" t="n">
-        <v>1393</v>
+        <v>17</v>
       </c>
       <c r="D2" t="n">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="E2" t="n">
-        <v>84</v>
+        <v>86</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>2</v>
+        <v>53</v>
       </c>
       <c r="B3" t="n">
-        <v>193</v>
+        <v>847</v>
       </c>
       <c r="C3" t="n">
-        <v>1380</v>
+        <v>131</v>
       </c>
       <c r="D3" t="n">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="E3" t="n">
-        <v>78</v>
+        <v>107</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>3</v>
+        <v>46</v>
       </c>
       <c r="B4" t="n">
-        <v>520</v>
+        <v>852</v>
       </c>
       <c r="C4" t="n">
-        <v>1376</v>
+        <v>259</v>
       </c>
       <c r="D4" t="n">
-        <v>46</v>
+        <v>61</v>
       </c>
       <c r="E4" t="n">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>4</v>
+        <v>59</v>
       </c>
       <c r="B5" t="n">
-        <v>355</v>
+        <v>682</v>
       </c>
       <c r="C5" t="n">
-        <v>1362</v>
+        <v>0</v>
       </c>
       <c r="D5" t="n">
-        <v>66</v>
+        <v>88</v>
       </c>
       <c r="E5" t="n">
-        <v>107</v>
+        <v>119</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>5</v>
+        <v>50</v>
       </c>
       <c r="B6" t="n">
-        <v>687</v>
+        <v>682</v>
       </c>
       <c r="C6" t="n">
-        <v>1265</v>
+        <v>140</v>
       </c>
       <c r="D6" t="n">
-        <v>61</v>
+        <v>80</v>
       </c>
       <c r="E6" t="n">
-        <v>97</v>
+        <v>100</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>6</v>
+        <v>44</v>
       </c>
       <c r="B7" t="n">
-        <v>32</v>
+        <v>676</v>
       </c>
       <c r="C7" t="n">
-        <v>1259</v>
+        <v>263</v>
       </c>
       <c r="D7" t="n">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="E7" t="n">
-        <v>82</v>
+        <v>96</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>7</v>
+        <v>41</v>
       </c>
       <c r="B8" t="n">
-        <v>190</v>
+        <v>685</v>
       </c>
       <c r="C8" t="n">
-        <v>1255</v>
+        <v>378</v>
       </c>
       <c r="D8" t="n">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E8" t="n">
-        <v>90</v>
+        <v>116</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>8</v>
+        <v>34</v>
       </c>
       <c r="B9" t="n">
-        <v>518</v>
+        <v>685</v>
       </c>
       <c r="C9" t="n">
-        <v>1250</v>
+        <v>517</v>
       </c>
       <c r="D9" t="n">
         <v>59</v>
       </c>
       <c r="E9" t="n">
-        <v>104</v>
+        <v>92</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>9</v>
+        <v>29</v>
       </c>
       <c r="B10" t="n">
-        <v>357</v>
+        <v>685</v>
       </c>
       <c r="C10" t="n">
-        <v>1240</v>
+        <v>643</v>
       </c>
       <c r="D10" t="n">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="E10" t="n">
-        <v>113</v>
+        <v>78</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="B11" t="n">
         <v>685</v>
       </c>
       <c r="C11" t="n">
-        <v>1140</v>
+        <v>756</v>
       </c>
       <c r="D11" t="n">
-        <v>70</v>
+        <v>76</v>
       </c>
       <c r="E11" t="n">
-        <v>90</v>
+        <v>100</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="B12" t="n">
-        <v>358</v>
+        <v>679</v>
       </c>
       <c r="C12" t="n">
-        <v>1128</v>
+        <v>882</v>
       </c>
       <c r="D12" t="n">
-        <v>66</v>
+        <v>82</v>
       </c>
       <c r="E12" t="n">
-        <v>94</v>
+        <v>111</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="B13" t="n">
-        <v>205</v>
+        <v>684</v>
       </c>
       <c r="C13" t="n">
-        <v>1128</v>
+        <v>1022</v>
       </c>
       <c r="D13" t="n">
-        <v>39</v>
+        <v>75</v>
       </c>
       <c r="E13" t="n">
-        <v>95</v>
+        <v>83</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B14" t="n">
-        <v>25</v>
+        <v>685</v>
       </c>
       <c r="C14" t="n">
-        <v>1120</v>
+        <v>1140</v>
       </c>
       <c r="D14" t="n">
-        <v>81</v>
+        <v>70</v>
       </c>
       <c r="E14" t="n">
-        <v>117</v>
+        <v>90</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="B15" t="n">
-        <v>516</v>
+        <v>687</v>
       </c>
       <c r="C15" t="n">
-        <v>1116</v>
+        <v>1265</v>
       </c>
       <c r="D15" t="n">
-        <v>76</v>
+        <v>61</v>
       </c>
       <c r="E15" t="n">
-        <v>119</v>
+        <v>97</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="B16" t="n">
-        <v>684</v>
+        <v>686</v>
       </c>
       <c r="C16" t="n">
-        <v>1022</v>
+        <v>1393</v>
       </c>
       <c r="D16" t="n">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="E16" t="n">
-        <v>83</v>
+        <v>84</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>16</v>
+        <v>57</v>
       </c>
       <c r="B17" t="n">
-        <v>198</v>
+        <v>523</v>
       </c>
       <c r="C17" t="n">
-        <v>1013</v>
+        <v>10</v>
       </c>
       <c r="D17" t="n">
-        <v>65</v>
+        <v>72</v>
       </c>
       <c r="E17" t="n">
-        <v>83</v>
+        <v>111</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>17</v>
+        <v>49</v>
       </c>
       <c r="B18" t="n">
-        <v>362</v>
+        <v>527</v>
       </c>
       <c r="C18" t="n">
-        <v>1006</v>
+        <v>142</v>
       </c>
       <c r="D18" t="n">
-        <v>59</v>
+        <v>70</v>
       </c>
       <c r="E18" t="n">
-        <v>99</v>
+        <v>93</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>18</v>
+        <v>47</v>
       </c>
       <c r="B19" t="n">
-        <v>22</v>
+        <v>516</v>
       </c>
       <c r="C19" t="n">
-        <v>1001</v>
+        <v>254</v>
       </c>
       <c r="D19" t="n">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="E19" t="n">
-        <v>92</v>
+        <v>110</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>19</v>
+        <v>38</v>
       </c>
       <c r="B20" t="n">
-        <v>359</v>
+        <v>523</v>
       </c>
       <c r="C20" t="n">
-        <v>890</v>
+        <v>393</v>
       </c>
       <c r="D20" t="n">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="E20" t="n">
-        <v>98</v>
+        <v>87</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>20</v>
+        <v>33</v>
       </c>
       <c r="B21" t="n">
-        <v>679</v>
+        <v>520</v>
       </c>
       <c r="C21" t="n">
-        <v>882</v>
+        <v>520</v>
       </c>
       <c r="D21" t="n">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="E21" t="n">
-        <v>111</v>
+        <v>79</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>21</v>
+        <v>32</v>
       </c>
       <c r="B22" t="n">
-        <v>29</v>
+        <v>535</v>
       </c>
       <c r="C22" t="n">
-        <v>882</v>
+        <v>620</v>
       </c>
       <c r="D22" t="n">
-        <v>79</v>
+        <v>42</v>
       </c>
       <c r="E22" t="n">
-        <v>84</v>
+        <v>67</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="n">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="B23" t="n">
-        <v>189</v>
+        <v>523</v>
       </c>
       <c r="C23" t="n">
-        <v>879</v>
+        <v>691</v>
       </c>
       <c r="D23" t="n">
-        <v>73</v>
+        <v>58</v>
       </c>
       <c r="E23" t="n">
-        <v>100</v>
+        <v>58</v>
       </c>
     </row>
     <row r="24">
@@ -853,271 +853,271 @@
     </row>
     <row r="25">
       <c r="A25" t="n">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="B25" t="n">
-        <v>33</v>
+        <v>516</v>
       </c>
       <c r="C25" t="n">
-        <v>762</v>
+        <v>1116</v>
       </c>
       <c r="D25" t="n">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="E25" t="n">
-        <v>84</v>
+        <v>119</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="n">
-        <v>25</v>
+        <v>8</v>
       </c>
       <c r="B26" t="n">
-        <v>685</v>
+        <v>518</v>
       </c>
       <c r="C26" t="n">
-        <v>756</v>
+        <v>1250</v>
       </c>
       <c r="D26" t="n">
-        <v>76</v>
+        <v>59</v>
       </c>
       <c r="E26" t="n">
-        <v>100</v>
+        <v>104</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="n">
-        <v>26</v>
+        <v>3</v>
       </c>
       <c r="B27" t="n">
-        <v>360</v>
+        <v>520</v>
       </c>
       <c r="C27" t="n">
-        <v>752</v>
+        <v>1376</v>
       </c>
       <c r="D27" t="n">
-        <v>80</v>
+        <v>46</v>
       </c>
       <c r="E27" t="n">
-        <v>113</v>
+        <v>93</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="n">
-        <v>27</v>
+        <v>58</v>
       </c>
       <c r="B28" t="n">
-        <v>523</v>
+        <v>368</v>
       </c>
       <c r="C28" t="n">
-        <v>691</v>
+        <v>10</v>
       </c>
       <c r="D28" t="n">
-        <v>58</v>
+        <v>78</v>
       </c>
       <c r="E28" t="n">
-        <v>58</v>
+        <v>116</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="n">
-        <v>28</v>
+        <v>51</v>
       </c>
       <c r="B29" t="n">
-        <v>194</v>
+        <v>355</v>
       </c>
       <c r="C29" t="n">
-        <v>655</v>
+        <v>137</v>
       </c>
       <c r="D29" t="n">
-        <v>70</v>
+        <v>89</v>
       </c>
       <c r="E29" t="n">
-        <v>73</v>
+        <v>100</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="n">
-        <v>29</v>
+        <v>43</v>
       </c>
       <c r="B30" t="n">
-        <v>685</v>
+        <v>361</v>
       </c>
       <c r="C30" t="n">
-        <v>643</v>
+        <v>265</v>
       </c>
       <c r="D30" t="n">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="E30" t="n">
-        <v>78</v>
+        <v>103</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="n">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="B31" t="n">
-        <v>35</v>
+        <v>370</v>
       </c>
       <c r="C31" t="n">
-        <v>633</v>
+        <v>389</v>
       </c>
       <c r="D31" t="n">
-        <v>73</v>
+        <v>65</v>
       </c>
       <c r="E31" t="n">
-        <v>96</v>
+        <v>81</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="n">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="B32" t="n">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="C32" t="n">
-        <v>625</v>
+        <v>502</v>
       </c>
       <c r="D32" t="n">
-        <v>61</v>
+        <v>67</v>
       </c>
       <c r="E32" t="n">
-        <v>108</v>
+        <v>94</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="n">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B33" t="n">
-        <v>535</v>
+        <v>366</v>
       </c>
       <c r="C33" t="n">
-        <v>620</v>
+        <v>625</v>
       </c>
       <c r="D33" t="n">
-        <v>42</v>
+        <v>61</v>
       </c>
       <c r="E33" t="n">
-        <v>67</v>
+        <v>108</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="n">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="B34" t="n">
-        <v>520</v>
+        <v>360</v>
       </c>
       <c r="C34" t="n">
-        <v>520</v>
+        <v>752</v>
       </c>
       <c r="D34" t="n">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="E34" t="n">
-        <v>79</v>
+        <v>113</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="n">
-        <v>34</v>
+        <v>19</v>
       </c>
       <c r="B35" t="n">
-        <v>685</v>
+        <v>359</v>
       </c>
       <c r="C35" t="n">
-        <v>517</v>
+        <v>890</v>
       </c>
       <c r="D35" t="n">
-        <v>59</v>
+        <v>79</v>
       </c>
       <c r="E35" t="n">
-        <v>92</v>
+        <v>98</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="n">
-        <v>35</v>
+        <v>17</v>
       </c>
       <c r="B36" t="n">
-        <v>189</v>
+        <v>362</v>
       </c>
       <c r="C36" t="n">
-        <v>512</v>
+        <v>1006</v>
       </c>
       <c r="D36" t="n">
-        <v>75</v>
+        <v>59</v>
       </c>
       <c r="E36" t="n">
-        <v>87</v>
+        <v>99</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="n">
-        <v>36</v>
+        <v>11</v>
       </c>
       <c r="B37" t="n">
-        <v>41</v>
+        <v>358</v>
       </c>
       <c r="C37" t="n">
-        <v>509</v>
+        <v>1128</v>
       </c>
       <c r="D37" t="n">
-        <v>42</v>
+        <v>66</v>
       </c>
       <c r="E37" t="n">
-        <v>92</v>
+        <v>94</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="n">
-        <v>37</v>
+        <v>9</v>
       </c>
       <c r="B38" t="n">
-        <v>364</v>
+        <v>357</v>
       </c>
       <c r="C38" t="n">
-        <v>502</v>
+        <v>1240</v>
       </c>
       <c r="D38" t="n">
-        <v>67</v>
+        <v>80</v>
       </c>
       <c r="E38" t="n">
-        <v>94</v>
+        <v>113</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="n">
-        <v>38</v>
+        <v>4</v>
       </c>
       <c r="B39" t="n">
-        <v>523</v>
+        <v>355</v>
       </c>
       <c r="C39" t="n">
-        <v>393</v>
+        <v>1362</v>
       </c>
       <c r="D39" t="n">
-        <v>76</v>
+        <v>66</v>
       </c>
       <c r="E39" t="n">
-        <v>87</v>
+        <v>107</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="n">
-        <v>39</v>
+        <v>54</v>
       </c>
       <c r="B40" t="n">
-        <v>34</v>
+        <v>190</v>
       </c>
       <c r="C40" t="n">
-        <v>392</v>
+        <v>21</v>
       </c>
       <c r="D40" t="n">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="E40" t="n">
         <v>86</v>
@@ -1125,342 +1125,342 @@
     </row>
     <row r="41">
       <c r="A41" t="n">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="B41" t="n">
-        <v>370</v>
+        <v>193</v>
       </c>
       <c r="C41" t="n">
-        <v>389</v>
+        <v>145</v>
       </c>
       <c r="D41" t="n">
-        <v>65</v>
+        <v>75</v>
       </c>
       <c r="E41" t="n">
-        <v>81</v>
+        <v>90</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="n">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B42" t="n">
-        <v>685</v>
+        <v>190</v>
       </c>
       <c r="C42" t="n">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="D42" t="n">
-        <v>74</v>
+        <v>80</v>
       </c>
       <c r="E42" t="n">
-        <v>116</v>
+        <v>108</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="n">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="B43" t="n">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C43" t="n">
-        <v>377</v>
+        <v>512</v>
       </c>
       <c r="D43" t="n">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="E43" t="n">
-        <v>108</v>
+        <v>87</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="n">
-        <v>43</v>
+        <v>28</v>
       </c>
       <c r="B44" t="n">
-        <v>361</v>
+        <v>194</v>
       </c>
       <c r="C44" t="n">
-        <v>265</v>
+        <v>655</v>
       </c>
       <c r="D44" t="n">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="E44" t="n">
-        <v>103</v>
+        <v>73</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="n">
-        <v>44</v>
+        <v>22</v>
       </c>
       <c r="B45" t="n">
-        <v>676</v>
+        <v>189</v>
       </c>
       <c r="C45" t="n">
-        <v>263</v>
+        <v>879</v>
       </c>
       <c r="D45" t="n">
-        <v>90</v>
+        <v>73</v>
       </c>
       <c r="E45" t="n">
-        <v>96</v>
+        <v>100</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="n">
-        <v>45</v>
+        <v>16</v>
       </c>
       <c r="B46" t="n">
-        <v>27</v>
+        <v>198</v>
       </c>
       <c r="C46" t="n">
-        <v>261</v>
+        <v>1013</v>
       </c>
       <c r="D46" t="n">
-        <v>87</v>
+        <v>65</v>
       </c>
       <c r="E46" t="n">
-        <v>110</v>
+        <v>83</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="n">
-        <v>46</v>
+        <v>12</v>
       </c>
       <c r="B47" t="n">
-        <v>852</v>
+        <v>205</v>
       </c>
       <c r="C47" t="n">
-        <v>259</v>
+        <v>1128</v>
       </c>
       <c r="D47" t="n">
-        <v>61</v>
+        <v>39</v>
       </c>
       <c r="E47" t="n">
-        <v>104</v>
+        <v>95</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="n">
-        <v>47</v>
+        <v>7</v>
       </c>
       <c r="B48" t="n">
-        <v>516</v>
+        <v>190</v>
       </c>
       <c r="C48" t="n">
-        <v>254</v>
+        <v>1255</v>
       </c>
       <c r="D48" t="n">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="E48" t="n">
-        <v>110</v>
+        <v>90</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="n">
-        <v>48</v>
+        <v>2</v>
       </c>
       <c r="B49" t="n">
         <v>193</v>
       </c>
       <c r="C49" t="n">
-        <v>145</v>
+        <v>1380</v>
       </c>
       <c r="D49" t="n">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E49" t="n">
-        <v>90</v>
+        <v>78</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="n">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="B50" t="n">
-        <v>527</v>
+        <v>31</v>
       </c>
       <c r="C50" t="n">
-        <v>142</v>
+        <v>19</v>
       </c>
       <c r="D50" t="n">
-        <v>70</v>
+        <v>82</v>
       </c>
       <c r="E50" t="n">
-        <v>93</v>
+        <v>83</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="n">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="B51" t="n">
-        <v>682</v>
+        <v>27</v>
       </c>
       <c r="C51" t="n">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="D51" t="n">
-        <v>80</v>
+        <v>88</v>
       </c>
       <c r="E51" t="n">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="n">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="B52" t="n">
-        <v>355</v>
+        <v>27</v>
       </c>
       <c r="C52" t="n">
-        <v>137</v>
+        <v>261</v>
       </c>
       <c r="D52" t="n">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="E52" t="n">
-        <v>100</v>
+        <v>110</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="n">
-        <v>52</v>
+        <v>39</v>
       </c>
       <c r="B53" t="n">
-        <v>27</v>
+        <v>34</v>
       </c>
       <c r="C53" t="n">
-        <v>136</v>
+        <v>392</v>
       </c>
       <c r="D53" t="n">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E53" t="n">
-        <v>99</v>
+        <v>86</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="n">
-        <v>53</v>
+        <v>36</v>
       </c>
       <c r="B54" t="n">
-        <v>847</v>
+        <v>41</v>
       </c>
       <c r="C54" t="n">
-        <v>131</v>
+        <v>509</v>
       </c>
       <c r="D54" t="n">
-        <v>79</v>
+        <v>42</v>
       </c>
       <c r="E54" t="n">
-        <v>107</v>
+        <v>92</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="n">
-        <v>54</v>
+        <v>30</v>
       </c>
       <c r="B55" t="n">
-        <v>190</v>
+        <v>35</v>
       </c>
       <c r="C55" t="n">
-        <v>21</v>
+        <v>633</v>
       </c>
       <c r="D55" t="n">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="E55" t="n">
-        <v>86</v>
+        <v>96</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="n">
-        <v>55</v>
+        <v>24</v>
       </c>
       <c r="B56" t="n">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C56" t="n">
-        <v>19</v>
+        <v>762</v>
       </c>
       <c r="D56" t="n">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="E56" t="n">
-        <v>83</v>
+        <v>84</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="n">
-        <v>56</v>
+        <v>21</v>
       </c>
       <c r="B57" t="n">
-        <v>847</v>
+        <v>29</v>
       </c>
       <c r="C57" t="n">
-        <v>17</v>
+        <v>882</v>
       </c>
       <c r="D57" t="n">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="E57" t="n">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="n">
-        <v>57</v>
+        <v>18</v>
       </c>
       <c r="B58" t="n">
-        <v>523</v>
+        <v>22</v>
       </c>
       <c r="C58" t="n">
-        <v>10</v>
+        <v>1001</v>
       </c>
       <c r="D58" t="n">
-        <v>72</v>
+        <v>85</v>
       </c>
       <c r="E58" t="n">
-        <v>111</v>
+        <v>92</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="n">
-        <v>58</v>
+        <v>13</v>
       </c>
       <c r="B59" t="n">
-        <v>368</v>
+        <v>25</v>
       </c>
       <c r="C59" t="n">
-        <v>10</v>
+        <v>1120</v>
       </c>
       <c r="D59" t="n">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="E59" t="n">
-        <v>116</v>
+        <v>117</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="n">
-        <v>59</v>
+        <v>6</v>
       </c>
       <c r="B60" t="n">
-        <v>682</v>
+        <v>32</v>
       </c>
       <c r="C60" t="n">
-        <v>0</v>
+        <v>1259</v>
       </c>
       <c r="D60" t="n">
         <v>88</v>
       </c>
       <c r="E60" t="n">
-        <v>119</v>
+        <v>82</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
minor modificcation on character 9
</commit_message>
<xml_diff>
--- a/character9/character9_boxes_location.xlsx
+++ b/character9/character9_boxes_location.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E69"/>
+  <dimension ref="A1:E68"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -462,13 +462,13 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B2" t="n">
         <v>847</v>
       </c>
       <c r="C2" t="n">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D2" t="n">
         <v>77</v>
@@ -479,13 +479,13 @@
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B3" t="n">
         <v>847</v>
       </c>
       <c r="C3" t="n">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="D3" t="n">
         <v>79</v>
@@ -496,13 +496,13 @@
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B4" t="n">
         <v>852</v>
       </c>
       <c r="C4" t="n">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="D4" t="n">
         <v>61</v>
@@ -513,13 +513,13 @@
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B5" t="n">
         <v>852</v>
       </c>
       <c r="C5" t="n">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="D5" t="n">
         <v>67</v>
@@ -530,13 +530,13 @@
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B6" t="n">
         <v>853</v>
       </c>
       <c r="C6" t="n">
-        <v>428</v>
+        <v>429</v>
       </c>
       <c r="D6" t="n">
         <v>65</v>
@@ -547,13 +547,13 @@
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B7" t="n">
         <v>855</v>
       </c>
       <c r="C7" t="n">
-        <v>458</v>
+        <v>459</v>
       </c>
       <c r="D7" t="n">
         <v>66</v>
@@ -564,7 +564,7 @@
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B8" t="n">
         <v>682</v>
@@ -576,18 +576,18 @@
         <v>88</v>
       </c>
       <c r="E8" t="n">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B9" t="n">
         <v>682</v>
       </c>
       <c r="C9" t="n">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="D9" t="n">
         <v>80</v>
@@ -598,13 +598,13 @@
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B10" t="n">
         <v>676</v>
       </c>
       <c r="C10" t="n">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="D10" t="n">
         <v>90</v>
@@ -615,13 +615,13 @@
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B11" t="n">
         <v>685</v>
       </c>
       <c r="C11" t="n">
-        <v>377</v>
+        <v>378</v>
       </c>
       <c r="D11" t="n">
         <v>74</v>
@@ -632,13 +632,13 @@
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B12" t="n">
         <v>685</v>
       </c>
       <c r="C12" t="n">
-        <v>516</v>
+        <v>517</v>
       </c>
       <c r="D12" t="n">
         <v>59</v>
@@ -649,13 +649,13 @@
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B13" t="n">
         <v>685</v>
       </c>
       <c r="C13" t="n">
-        <v>642</v>
+        <v>643</v>
       </c>
       <c r="D13" t="n">
         <v>74</v>
@@ -672,7 +672,7 @@
         <v>685</v>
       </c>
       <c r="C14" t="n">
-        <v>755</v>
+        <v>756</v>
       </c>
       <c r="D14" t="n">
         <v>76</v>
@@ -689,7 +689,7 @@
         <v>679</v>
       </c>
       <c r="C15" t="n">
-        <v>881</v>
+        <v>882</v>
       </c>
       <c r="D15" t="n">
         <v>82</v>
@@ -706,7 +706,7 @@
         <v>684</v>
       </c>
       <c r="C16" t="n">
-        <v>1021</v>
+        <v>1022</v>
       </c>
       <c r="D16" t="n">
         <v>75</v>
@@ -723,7 +723,7 @@
         <v>685</v>
       </c>
       <c r="C17" t="n">
-        <v>1139</v>
+        <v>1140</v>
       </c>
       <c r="D17" t="n">
         <v>70</v>
@@ -740,7 +740,7 @@
         <v>687</v>
       </c>
       <c r="C18" t="n">
-        <v>1264</v>
+        <v>1265</v>
       </c>
       <c r="D18" t="n">
         <v>61</v>
@@ -757,24 +757,24 @@
         <v>686</v>
       </c>
       <c r="C19" t="n">
-        <v>1392</v>
+        <v>1393</v>
       </c>
       <c r="D19" t="n">
         <v>73</v>
       </c>
       <c r="E19" t="n">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B20" t="n">
         <v>523</v>
       </c>
       <c r="C20" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D20" t="n">
         <v>72</v>
@@ -785,13 +785,13 @@
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B21" t="n">
         <v>527</v>
       </c>
       <c r="C21" t="n">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="D21" t="n">
         <v>70</v>
@@ -802,13 +802,13 @@
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B22" t="n">
         <v>516</v>
       </c>
       <c r="C22" t="n">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="D22" t="n">
         <v>81</v>
@@ -819,13 +819,13 @@
     </row>
     <row r="23">
       <c r="A23" t="n">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B23" t="n">
         <v>523</v>
       </c>
       <c r="C23" t="n">
-        <v>392</v>
+        <v>393</v>
       </c>
       <c r="D23" t="n">
         <v>76</v>
@@ -836,13 +836,13 @@
     </row>
     <row r="24">
       <c r="A24" t="n">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B24" t="n">
         <v>520</v>
       </c>
       <c r="C24" t="n">
-        <v>519</v>
+        <v>520</v>
       </c>
       <c r="D24" t="n">
         <v>84</v>
@@ -853,407 +853,407 @@
     </row>
     <row r="25">
       <c r="A25" t="n">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B25" t="n">
-        <v>535</v>
+        <v>523</v>
       </c>
       <c r="C25" t="n">
-        <v>619</v>
+        <v>620</v>
       </c>
       <c r="D25" t="n">
-        <v>42</v>
+        <v>58</v>
       </c>
       <c r="E25" t="n">
-        <v>67</v>
+        <v>129</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="n">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="B26" t="n">
-        <v>523</v>
+        <v>519</v>
       </c>
       <c r="C26" t="n">
-        <v>690</v>
+        <v>766</v>
       </c>
       <c r="D26" t="n">
-        <v>58</v>
+        <v>66</v>
       </c>
       <c r="E26" t="n">
-        <v>58</v>
+        <v>95</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="n">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="B27" t="n">
-        <v>519</v>
+        <v>521</v>
       </c>
       <c r="C27" t="n">
-        <v>765</v>
+        <v>1013</v>
       </c>
       <c r="D27" t="n">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="E27" t="n">
-        <v>95</v>
+        <v>11</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="n">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B28" t="n">
-        <v>521</v>
+        <v>523</v>
       </c>
       <c r="C28" t="n">
-        <v>1012</v>
+        <v>1043</v>
       </c>
       <c r="D28" t="n">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="E28" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="n">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B29" t="n">
         <v>523</v>
       </c>
       <c r="C29" t="n">
-        <v>1042</v>
+        <v>1072</v>
       </c>
       <c r="D29" t="n">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="E29" t="n">
-        <v>10</v>
+        <v>13</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="n">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B30" t="n">
-        <v>523</v>
+        <v>516</v>
       </c>
       <c r="C30" t="n">
-        <v>1071</v>
+        <v>1116</v>
       </c>
       <c r="D30" t="n">
-        <v>67</v>
+        <v>76</v>
       </c>
       <c r="E30" t="n">
-        <v>13</v>
+        <v>119</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="n">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="B31" t="n">
-        <v>516</v>
+        <v>518</v>
       </c>
       <c r="C31" t="n">
-        <v>1115</v>
+        <v>1250</v>
       </c>
       <c r="D31" t="n">
-        <v>76</v>
+        <v>59</v>
       </c>
       <c r="E31" t="n">
-        <v>119</v>
+        <v>104</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="n">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="B32" t="n">
-        <v>518</v>
+        <v>520</v>
       </c>
       <c r="C32" t="n">
-        <v>1249</v>
+        <v>1376</v>
       </c>
       <c r="D32" t="n">
-        <v>59</v>
+        <v>46</v>
       </c>
       <c r="E32" t="n">
-        <v>104</v>
+        <v>93</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="n">
-        <v>3</v>
+        <v>66</v>
       </c>
       <c r="B33" t="n">
-        <v>520</v>
+        <v>368</v>
       </c>
       <c r="C33" t="n">
-        <v>1375</v>
+        <v>10</v>
       </c>
       <c r="D33" t="n">
-        <v>46</v>
+        <v>78</v>
       </c>
       <c r="E33" t="n">
-        <v>93</v>
+        <v>116</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="n">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="B34" t="n">
-        <v>368</v>
+        <v>355</v>
       </c>
       <c r="C34" t="n">
-        <v>9</v>
+        <v>137</v>
       </c>
       <c r="D34" t="n">
-        <v>78</v>
+        <v>89</v>
       </c>
       <c r="E34" t="n">
-        <v>116</v>
+        <v>100</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="n">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="B35" t="n">
-        <v>355</v>
+        <v>361</v>
       </c>
       <c r="C35" t="n">
-        <v>136</v>
+        <v>265</v>
       </c>
       <c r="D35" t="n">
-        <v>89</v>
+        <v>76</v>
       </c>
       <c r="E35" t="n">
-        <v>100</v>
+        <v>103</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="n">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="B36" t="n">
-        <v>361</v>
+        <v>370</v>
       </c>
       <c r="C36" t="n">
-        <v>264</v>
+        <v>389</v>
       </c>
       <c r="D36" t="n">
-        <v>76</v>
+        <v>65</v>
       </c>
       <c r="E36" t="n">
-        <v>103</v>
+        <v>81</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="n">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="B37" t="n">
-        <v>370</v>
+        <v>364</v>
       </c>
       <c r="C37" t="n">
-        <v>388</v>
+        <v>502</v>
       </c>
       <c r="D37" t="n">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="E37" t="n">
-        <v>81</v>
+        <v>94</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="n">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="B38" t="n">
-        <v>364</v>
+        <v>366</v>
       </c>
       <c r="C38" t="n">
-        <v>501</v>
+        <v>625</v>
       </c>
       <c r="D38" t="n">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="E38" t="n">
-        <v>94</v>
+        <v>108</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="n">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="B39" t="n">
-        <v>366</v>
+        <v>360</v>
       </c>
       <c r="C39" t="n">
-        <v>624</v>
+        <v>752</v>
       </c>
       <c r="D39" t="n">
-        <v>61</v>
+        <v>80</v>
       </c>
       <c r="E39" t="n">
-        <v>108</v>
+        <v>113</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="n">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="B40" t="n">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="C40" t="n">
-        <v>751</v>
+        <v>890</v>
       </c>
       <c r="D40" t="n">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E40" t="n">
-        <v>113</v>
+        <v>98</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="n">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B41" t="n">
-        <v>359</v>
+        <v>362</v>
       </c>
       <c r="C41" t="n">
-        <v>889</v>
+        <v>1006</v>
       </c>
       <c r="D41" t="n">
-        <v>79</v>
+        <v>59</v>
       </c>
       <c r="E41" t="n">
-        <v>98</v>
+        <v>99</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="n">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="B42" t="n">
-        <v>362</v>
+        <v>358</v>
       </c>
       <c r="C42" t="n">
-        <v>1005</v>
+        <v>1128</v>
       </c>
       <c r="D42" t="n">
-        <v>59</v>
+        <v>66</v>
       </c>
       <c r="E42" t="n">
-        <v>99</v>
+        <v>94</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="n">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B43" t="n">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="C43" t="n">
-        <v>1127</v>
+        <v>1240</v>
       </c>
       <c r="D43" t="n">
-        <v>66</v>
+        <v>80</v>
       </c>
       <c r="E43" t="n">
-        <v>94</v>
+        <v>113</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="n">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="B44" t="n">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="C44" t="n">
-        <v>1239</v>
+        <v>1362</v>
       </c>
       <c r="D44" t="n">
-        <v>80</v>
+        <v>66</v>
       </c>
       <c r="E44" t="n">
-        <v>113</v>
+        <v>107</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="n">
-        <v>4</v>
+        <v>62</v>
       </c>
       <c r="B45" t="n">
-        <v>355</v>
+        <v>190</v>
       </c>
       <c r="C45" t="n">
-        <v>1361</v>
+        <v>21</v>
       </c>
       <c r="D45" t="n">
-        <v>66</v>
+        <v>80</v>
       </c>
       <c r="E45" t="n">
-        <v>107</v>
+        <v>86</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="n">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="B46" t="n">
-        <v>190</v>
+        <v>193</v>
       </c>
       <c r="C46" t="n">
-        <v>20</v>
+        <v>145</v>
       </c>
       <c r="D46" t="n">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="E46" t="n">
-        <v>86</v>
+        <v>90</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="n">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="B47" t="n">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="C47" t="n">
-        <v>144</v>
+        <v>270</v>
       </c>
       <c r="D47" t="n">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="E47" t="n">
-        <v>90</v>
+        <v>10</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="n">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B48" t="n">
-        <v>194</v>
+        <v>197</v>
       </c>
       <c r="C48" t="n">
-        <v>269</v>
+        <v>300</v>
       </c>
       <c r="D48" t="n">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="E48" t="n">
         <v>10</v>
@@ -1261,16 +1261,16 @@
     </row>
     <row r="49">
       <c r="A49" t="n">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B49" t="n">
         <v>197</v>
       </c>
       <c r="C49" t="n">
-        <v>299</v>
+        <v>333</v>
       </c>
       <c r="D49" t="n">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="E49" t="n">
         <v>10</v>
@@ -1278,271 +1278,271 @@
     </row>
     <row r="50">
       <c r="A50" t="n">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B50" t="n">
-        <v>197</v>
+        <v>190</v>
       </c>
       <c r="C50" t="n">
-        <v>332</v>
+        <v>377</v>
       </c>
       <c r="D50" t="n">
-        <v>68</v>
+        <v>80</v>
       </c>
       <c r="E50" t="n">
-        <v>10</v>
+        <v>108</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="n">
-        <v>48</v>
+        <v>37</v>
       </c>
       <c r="B51" t="n">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C51" t="n">
-        <v>376</v>
+        <v>512</v>
       </c>
       <c r="D51" t="n">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="E51" t="n">
-        <v>108</v>
+        <v>87</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="n">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="B52" t="n">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="C52" t="n">
-        <v>511</v>
+        <v>637</v>
       </c>
       <c r="D52" t="n">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="E52" t="n">
-        <v>87</v>
+        <v>91</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="n">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="B53" t="n">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="C53" t="n">
-        <v>636</v>
+        <v>879</v>
       </c>
       <c r="D53" t="n">
         <v>73</v>
       </c>
       <c r="E53" t="n">
-        <v>91</v>
+        <v>100</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="n">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="B54" t="n">
-        <v>189</v>
+        <v>198</v>
       </c>
       <c r="C54" t="n">
-        <v>878</v>
+        <v>1013</v>
       </c>
       <c r="D54" t="n">
-        <v>73</v>
+        <v>65</v>
       </c>
       <c r="E54" t="n">
-        <v>100</v>
+        <v>83</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="n">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="B55" t="n">
-        <v>198</v>
+        <v>205</v>
       </c>
       <c r="C55" t="n">
-        <v>1012</v>
+        <v>1128</v>
       </c>
       <c r="D55" t="n">
-        <v>65</v>
+        <v>39</v>
       </c>
       <c r="E55" t="n">
-        <v>83</v>
+        <v>95</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="n">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="B56" t="n">
-        <v>205</v>
+        <v>190</v>
       </c>
       <c r="C56" t="n">
-        <v>1127</v>
+        <v>1255</v>
       </c>
       <c r="D56" t="n">
-        <v>39</v>
+        <v>76</v>
       </c>
       <c r="E56" t="n">
-        <v>95</v>
+        <v>90</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="n">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B57" t="n">
-        <v>190</v>
+        <v>193</v>
       </c>
       <c r="C57" t="n">
-        <v>1254</v>
+        <v>1380</v>
       </c>
       <c r="D57" t="n">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E57" t="n">
-        <v>90</v>
+        <v>78</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="n">
-        <v>2</v>
+        <v>63</v>
       </c>
       <c r="B58" t="n">
-        <v>193</v>
+        <v>31</v>
       </c>
       <c r="C58" t="n">
-        <v>1379</v>
+        <v>19</v>
       </c>
       <c r="D58" t="n">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="E58" t="n">
-        <v>78</v>
+        <v>83</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="n">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="B59" t="n">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C59" t="n">
-        <v>18</v>
+        <v>136</v>
       </c>
       <c r="D59" t="n">
-        <v>82</v>
+        <v>88</v>
       </c>
       <c r="E59" t="n">
-        <v>83</v>
+        <v>99</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="n">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="B60" t="n">
         <v>27</v>
       </c>
       <c r="C60" t="n">
-        <v>135</v>
+        <v>261</v>
       </c>
       <c r="D60" t="n">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E60" t="n">
-        <v>99</v>
+        <v>110</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="n">
-        <v>54</v>
+        <v>44</v>
       </c>
       <c r="B61" t="n">
-        <v>27</v>
+        <v>34</v>
       </c>
       <c r="C61" t="n">
-        <v>260</v>
+        <v>392</v>
       </c>
       <c r="D61" t="n">
         <v>87</v>
       </c>
       <c r="E61" t="n">
-        <v>110</v>
+        <v>86</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="n">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="B62" t="n">
-        <v>34</v>
+        <v>41</v>
       </c>
       <c r="C62" t="n">
-        <v>391</v>
+        <v>509</v>
       </c>
       <c r="D62" t="n">
-        <v>87</v>
+        <v>42</v>
       </c>
       <c r="E62" t="n">
-        <v>86</v>
+        <v>92</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="n">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="B63" t="n">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="C63" t="n">
-        <v>508</v>
+        <v>633</v>
       </c>
       <c r="D63" t="n">
-        <v>42</v>
+        <v>73</v>
       </c>
       <c r="E63" t="n">
-        <v>92</v>
+        <v>96</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="n">
+        <v>27</v>
+      </c>
+      <c r="B64" t="n">
         <v>33</v>
       </c>
-      <c r="B64" t="n">
-        <v>35</v>
-      </c>
       <c r="C64" t="n">
-        <v>632</v>
+        <v>762</v>
       </c>
       <c r="D64" t="n">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="E64" t="n">
-        <v>96</v>
+        <v>84</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="n">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B65" t="n">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C65" t="n">
-        <v>761</v>
+        <v>882</v>
       </c>
       <c r="D65" t="n">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="E65" t="n">
         <v>84</v>
@@ -1550,69 +1550,52 @@
     </row>
     <row r="66">
       <c r="A66" t="n">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B66" t="n">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="C66" t="n">
-        <v>881</v>
+        <v>1001</v>
       </c>
       <c r="D66" t="n">
-        <v>79</v>
+        <v>85</v>
       </c>
       <c r="E66" t="n">
-        <v>84</v>
+        <v>92</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="n">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="B67" t="n">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="C67" t="n">
-        <v>1000</v>
+        <v>1120</v>
       </c>
       <c r="D67" t="n">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="E67" t="n">
-        <v>92</v>
+        <v>117</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="n">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="B68" t="n">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="C68" t="n">
-        <v>1119</v>
+        <v>1259</v>
       </c>
       <c r="D68" t="n">
-        <v>81</v>
+        <v>88</v>
       </c>
       <c r="E68" t="n">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="69">
-      <c r="A69" t="n">
-        <v>6</v>
-      </c>
-      <c r="B69" t="n">
-        <v>32</v>
-      </c>
-      <c r="C69" t="n">
-        <v>1258</v>
-      </c>
-      <c r="D69" t="n">
-        <v>88</v>
-      </c>
-      <c r="E69" t="n">
         <v>82</v>
       </c>
     </row>

</xml_diff>